<commit_message>
MaJ ajout onglet panorama avec calcul DLR
</commit_message>
<xml_diff>
--- a/TaC/Regates/TQ/TQ_ResultatsFFV.xlsx
+++ b/TaC/Regates/TQ/TQ_ResultatsFFV.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="23715" windowHeight="11055" activeTab="9"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="23715" windowHeight="11055" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Vents" sheetId="9" r:id="rId1"/>
@@ -16,14 +16,15 @@
     <sheet name="2012A2" sheetId="6" r:id="rId7"/>
     <sheet name="2012A1" sheetId="7" r:id="rId8"/>
     <sheet name="2012M1" sheetId="8" r:id="rId9"/>
-    <sheet name="Feuil2" sheetId="10" r:id="rId10"/>
+    <sheet name="Figaro2" sheetId="10" r:id="rId10"/>
+    <sheet name="Panorama" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2578" uniqueCount="1097">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2628" uniqueCount="1141">
   <si>
     <t>place </t>
   </si>
@@ -3315,12 +3316,147 @@
   </si>
   <si>
     <t>Figaro TCC 1,105 / 1,092 /1,085 /1,066 / yuzu 1.046</t>
+  </si>
+  <si>
+    <t>Ofcet 32</t>
+  </si>
+  <si>
+    <t>jpk 10.10</t>
+  </si>
+  <si>
+    <t>jpk 10.80</t>
+  </si>
+  <si>
+    <t>MC 34</t>
+  </si>
+  <si>
+    <t>sf 3200</t>
+  </si>
+  <si>
+    <t>sf 3600</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Dep.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">€ </t>
+  </si>
+  <si>
+    <t>240K</t>
+  </si>
+  <si>
+    <t>bau</t>
+  </si>
+  <si>
+    <t>TE</t>
+  </si>
+  <si>
+    <t>Valer</t>
+  </si>
+  <si>
+    <t>Lombard</t>
+  </si>
+  <si>
+    <t>134K</t>
+  </si>
+  <si>
+    <t>123K</t>
+  </si>
+  <si>
+    <t>165K</t>
+  </si>
+  <si>
+    <t>Andrieux</t>
+  </si>
+  <si>
+    <t>103K</t>
+  </si>
+  <si>
+    <t>168K</t>
+  </si>
+  <si>
+    <t>Pogo 30</t>
+  </si>
+  <si>
+    <t>Pogo 36</t>
+  </si>
+  <si>
+    <t>Pogo 10.50</t>
+  </si>
+  <si>
+    <t>Finot-Conq</t>
+  </si>
+  <si>
+    <t>109K</t>
+  </si>
+  <si>
+    <t>160K</t>
+  </si>
+  <si>
+    <t>1,1 - 2,9</t>
+  </si>
+  <si>
+    <t>LF</t>
+  </si>
+  <si>
+    <t>1,1 - 2,80</t>
+  </si>
+  <si>
+    <t>lest</t>
+  </si>
+  <si>
+    <t>GV</t>
+  </si>
+  <si>
+    <t>avant</t>
+  </si>
+  <si>
+    <t>spi</t>
+  </si>
+  <si>
+    <t>85 (95 asy)</t>
+  </si>
+  <si>
+    <t>120 (105 asy)</t>
+  </si>
+  <si>
+    <t>Figaro 2</t>
+  </si>
+  <si>
+    <t>bau flot</t>
+  </si>
+  <si>
+    <t>120 asy</t>
+  </si>
+  <si>
+    <t>Figaro 1</t>
+  </si>
+  <si>
+    <t>Berret Finot</t>
+  </si>
+  <si>
+    <t>DLR</t>
+  </si>
+  <si>
+    <t>Bepox 9.90</t>
+  </si>
+  <si>
+    <t>FC12 de série</t>
+  </si>
+  <si>
+    <t>Finot</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3354,7 +3490,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -3362,12 +3498,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3385,6 +3536,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -18314,7 +18481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
@@ -18386,6 +18553,613 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:O15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="4.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="7" customWidth="1"/>
+    <col min="10" max="10" width="5.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="11" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>1108</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>1103</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>1124</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>1107</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>1133</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>1104</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>1126</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>1137</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>1127</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>1128</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E3" s="15">
+        <v>2</v>
+      </c>
+      <c r="F3" s="15">
+        <v>10.5</v>
+      </c>
+      <c r="G3" s="15">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="H3" s="15">
+        <v>3.46</v>
+      </c>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15">
+        <v>3.65</v>
+      </c>
+      <c r="K3" s="15">
+        <v>1.8</v>
+      </c>
+      <c r="L3" s="15">
+        <f>(J3*0.984) / (G3*3.28*0.01)^3</f>
+        <v>130.70823483587299</v>
+      </c>
+      <c r="M3" s="15">
+        <v>37</v>
+      </c>
+      <c r="N3" s="15">
+        <v>30</v>
+      </c>
+      <c r="O3" s="15">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="13" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>1111</v>
+      </c>
+      <c r="E4" s="15">
+        <v>2</v>
+      </c>
+      <c r="F4" s="15">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="G4" s="15">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="H4" s="15">
+        <v>3.45</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="K4" s="15">
+        <v>1.55</v>
+      </c>
+      <c r="L4" s="15">
+        <f t="shared" ref="L4:L15" si="0">(J4*0.984) / (G4*3.28*0.01)^3</f>
+        <v>156.69964030781534</v>
+      </c>
+      <c r="M4" s="15">
+        <v>31</v>
+      </c>
+      <c r="N4" s="15">
+        <v>27</v>
+      </c>
+      <c r="O4" s="15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="13" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E5" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="F5" s="15">
+        <v>9.77</v>
+      </c>
+      <c r="G5" s="15">
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="H5" s="15">
+        <v>3.48</v>
+      </c>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15">
+        <v>3.4</v>
+      </c>
+      <c r="K5" s="15">
+        <v>1.3</v>
+      </c>
+      <c r="L5" s="15">
+        <f t="shared" si="0"/>
+        <v>151.68901811665376</v>
+      </c>
+      <c r="M5" s="15">
+        <v>34</v>
+      </c>
+      <c r="N5" s="15">
+        <v>30</v>
+      </c>
+      <c r="O5" s="15">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>1112</v>
+      </c>
+      <c r="E6" s="15">
+        <v>2</v>
+      </c>
+      <c r="F6" s="15">
+        <v>10</v>
+      </c>
+      <c r="G6" s="15">
+        <v>8.76</v>
+      </c>
+      <c r="H6" s="15">
+        <v>3.39</v>
+      </c>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15">
+        <v>3.85</v>
+      </c>
+      <c r="K6" s="15">
+        <v>1.65</v>
+      </c>
+      <c r="L6" s="15">
+        <f t="shared" si="0"/>
+        <v>159.7062742699336</v>
+      </c>
+      <c r="M6" s="15">
+        <v>33</v>
+      </c>
+      <c r="N6" s="15">
+        <v>25</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>1116</v>
+      </c>
+      <c r="E7" s="15">
+        <v>2.13</v>
+      </c>
+      <c r="F7" s="15">
+        <v>10.8</v>
+      </c>
+      <c r="G7" s="15">
+        <v>9.5</v>
+      </c>
+      <c r="H7" s="15">
+        <v>3.55</v>
+      </c>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="K7" s="15">
+        <v>2</v>
+      </c>
+      <c r="L7" s="15">
+        <f t="shared" si="0"/>
+        <v>159.36715929838209</v>
+      </c>
+      <c r="M7" s="15">
+        <v>37</v>
+      </c>
+      <c r="N7" s="15">
+        <v>33</v>
+      </c>
+      <c r="O7" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>1113</v>
+      </c>
+      <c r="E8" s="15">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F8" s="15">
+        <v>10.8</v>
+      </c>
+      <c r="G8" s="15">
+        <v>9.4</v>
+      </c>
+      <c r="H8" s="15">
+        <v>3.65</v>
+      </c>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15">
+        <v>4.75</v>
+      </c>
+      <c r="K8" s="15">
+        <v>2.15</v>
+      </c>
+      <c r="L8" s="15">
+        <f t="shared" si="0"/>
+        <v>159.4716971374134</v>
+      </c>
+      <c r="M8" s="15">
+        <v>40</v>
+      </c>
+      <c r="N8" s="15">
+        <v>33</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F9" s="15">
+        <v>10.5</v>
+      </c>
+      <c r="G9" s="15">
+        <v>10.5</v>
+      </c>
+      <c r="H9" s="15">
+        <v>3.9</v>
+      </c>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15">
+        <v>3.6</v>
+      </c>
+      <c r="K9" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L9" s="15">
+        <f t="shared" si="0"/>
+        <v>86.717783909688649</v>
+      </c>
+      <c r="M9" s="15">
+        <v>37</v>
+      </c>
+      <c r="N9" s="15">
+        <v>34</v>
+      </c>
+      <c r="O9" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="13" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>1121</v>
+      </c>
+      <c r="E10" s="15">
+        <v>1.6</v>
+      </c>
+      <c r="F10" s="15">
+        <v>9.14</v>
+      </c>
+      <c r="G10" s="15">
+        <v>9.1</v>
+      </c>
+      <c r="H10" s="15">
+        <v>3.7</v>
+      </c>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15">
+        <v>2.8</v>
+      </c>
+      <c r="K10" s="15">
+        <v>0.95</v>
+      </c>
+      <c r="L10" s="15">
+        <f t="shared" si="0"/>
+        <v>103.61137130766168</v>
+      </c>
+      <c r="M10" s="15">
+        <v>34</v>
+      </c>
+      <c r="N10" s="15">
+        <v>26</v>
+      </c>
+      <c r="O10" s="15">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="13" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>1122</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>1123</v>
+      </c>
+      <c r="F11" s="15">
+        <v>10.8</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15">
+        <v>4</v>
+      </c>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15">
+        <v>4</v>
+      </c>
+      <c r="K11" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L11" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M11" s="15">
+        <v>45</v>
+      </c>
+      <c r="N11" s="15">
+        <v>29</v>
+      </c>
+      <c r="O11" s="16" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="13" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="15">
+        <v>2.4</v>
+      </c>
+      <c r="F12" s="15">
+        <v>9.9</v>
+      </c>
+      <c r="G12" s="15">
+        <v>9.9</v>
+      </c>
+      <c r="H12" s="15">
+        <v>3</v>
+      </c>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15">
+        <v>2.7</v>
+      </c>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15">
+        <f t="shared" si="0"/>
+        <v>77.594644484679435</v>
+      </c>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="16"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="13" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15">
+        <v>2.1</v>
+      </c>
+      <c r="F13" s="15">
+        <v>12</v>
+      </c>
+      <c r="G13" s="15">
+        <v>10.3</v>
+      </c>
+      <c r="H13" s="15">
+        <v>3.8</v>
+      </c>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15">
+        <v>4.3</v>
+      </c>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15">
+        <f t="shared" si="0"/>
+        <v>109.73125562960811</v>
+      </c>
+      <c r="M13" s="15">
+        <v>41</v>
+      </c>
+      <c r="N13" s="15">
+        <v>28</v>
+      </c>
+      <c r="O13" s="16"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="15">
+        <v>2.15</v>
+      </c>
+      <c r="F14" s="15">
+        <v>10.11</v>
+      </c>
+      <c r="G14" s="15">
+        <v>9.82</v>
+      </c>
+      <c r="H14" s="15">
+        <v>3.43</v>
+      </c>
+      <c r="I14" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="J14" s="15">
+        <v>3</v>
+      </c>
+      <c r="K14" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L14" s="15">
+        <f t="shared" si="0"/>
+        <v>88.340602856022727</v>
+      </c>
+      <c r="M14" s="15">
+        <v>38</v>
+      </c>
+      <c r="N14" s="15">
+        <v>30</v>
+      </c>
+      <c r="O14" s="15">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="13" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="15">
+        <v>1.8</v>
+      </c>
+      <c r="F15" s="15">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="G15" s="15">
+        <v>8.4</v>
+      </c>
+      <c r="H15" s="15">
+        <v>3.25</v>
+      </c>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="K15" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="L15" s="15">
+        <f t="shared" si="0"/>
+        <v>117.61852201292405</v>
+      </c>
+      <c r="M15" s="15">
+        <v>26</v>
+      </c>
+      <c r="N15" s="15">
+        <v>30</v>
+      </c>
+      <c r="O15" s="15">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
MAJ ajout TCC, --et bateau cible--
</commit_message>
<xml_diff>
--- a/TaC/Regates/TQ/TQ_ResultatsFFV.xlsx
+++ b/TaC/Regates/TQ/TQ_ResultatsFFV.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2628" uniqueCount="1141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2636" uniqueCount="1149">
   <si>
     <t>place </t>
   </si>
@@ -3448,16 +3448,41 @@
   </si>
   <si>
     <t>Finot</t>
+  </si>
+  <si>
+    <t>TCC -</t>
+  </si>
+  <si>
+    <t>TCC</t>
+  </si>
+  <si>
+    <t>TCC +</t>
+  </si>
+  <si>
+    <t>? 1.010</t>
+  </si>
+  <si>
+    <t>Sormiou 29</t>
+  </si>
+  <si>
+    <t>Philippot</t>
+  </si>
+  <si>
+    <t>105K</t>
+  </si>
+  <si>
+    <t>cible TQ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3477,6 +3502,21 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3518,7 +3558,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3552,6 +3592,18 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -18558,604 +18610,1335 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O15"/>
+  <dimension ref="A1:AN17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="4.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="7" customWidth="1"/>
-    <col min="10" max="10" width="5.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="4.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.28515625" customWidth="1"/>
+    <col min="19" max="39" width="6" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="11" t="s">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D1" s="7">
+        <v>2</v>
+      </c>
+      <c r="E1" s="7">
+        <v>10</v>
+      </c>
+      <c r="F1" s="7">
+        <v>9.5</v>
+      </c>
+      <c r="G1" s="7">
+        <v>3.45</v>
+      </c>
+      <c r="I1" s="7">
+        <v>3.4</v>
+      </c>
+      <c r="K1" s="15">
+        <f>(I1*0.984) / (F1*3.28*0.01)^3</f>
+        <v>110.58129420704061</v>
+      </c>
+      <c r="L1">
+        <v>30</v>
+      </c>
+      <c r="M1">
+        <v>23</v>
+      </c>
+      <c r="N1" s="7">
+        <v>92</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11" t="s">
         <v>1105</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="D3" s="12" t="s">
         <v>1108</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="E3" s="12" t="s">
         <v>1103</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="F3" s="12" t="s">
         <v>1124</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="G3" s="12" t="s">
         <v>1107</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="H3" s="12" t="s">
         <v>1133</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="I3" s="12" t="s">
         <v>1104</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="J3" s="12" t="s">
         <v>1126</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="K3" s="12" t="s">
         <v>1137</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="L3" s="12" t="s">
         <v>1127</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="M3" s="12" t="s">
         <v>1128</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="N3" s="12" t="s">
         <v>1129</v>
       </c>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+      <c r="O3" s="17" t="s">
+        <v>1141</v>
+      </c>
+      <c r="P3" s="17" t="s">
+        <v>1142</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>1100</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="B4" s="13" t="s">
         <v>1110</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="C4" s="14" t="s">
         <v>1106</v>
       </c>
-      <c r="E3" s="15">
+      <c r="D4" s="15">
         <v>2</v>
       </c>
-      <c r="F3" s="15">
+      <c r="E4" s="15">
         <v>10.5</v>
       </c>
-      <c r="G3" s="15">
+      <c r="F4" s="15">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H3" s="15">
+      <c r="G4" s="15">
         <v>3.46</v>
       </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15">
+      <c r="H4" s="15"/>
+      <c r="I4" s="15">
         <v>3.65</v>
       </c>
-      <c r="K3" s="15">
+      <c r="J4" s="15">
         <v>1.8</v>
       </c>
-      <c r="L3" s="15">
-        <f>(J3*0.984) / (G3*3.28*0.01)^3</f>
+      <c r="K4" s="15">
+        <f>(I4*0.984) / (F4*3.28*0.01)^3</f>
         <v>130.70823483587299</v>
       </c>
-      <c r="M3" s="15">
+      <c r="L4" s="15">
         <v>37</v>
       </c>
-      <c r="N3" s="15">
+      <c r="M4" s="15">
         <v>30</v>
       </c>
-      <c r="O3" s="15">
+      <c r="N4" s="15">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="O4" s="19">
+        <f>MIN(S4:AK4)</f>
+        <v>1.0429999999999999</v>
+      </c>
+      <c r="P4" s="19">
+        <f>MEDIAN(S4,AK4)</f>
+        <v>1.0429999999999999</v>
+      </c>
+      <c r="Q4" s="19">
+        <f>MAX(S4:AK4)</f>
+        <v>1.1439999999999999</v>
+      </c>
+      <c r="S4" s="18">
+        <v>1.0429999999999999</v>
+      </c>
+      <c r="T4" s="18">
+        <v>1.06</v>
+      </c>
+      <c r="U4" s="18">
+        <v>1.1439999999999999</v>
+      </c>
+      <c r="V4" s="20">
+        <v>1.0509999999999999</v>
+      </c>
+      <c r="W4" s="18"/>
+      <c r="X4" s="18"/>
+      <c r="Y4" s="18"/>
+      <c r="Z4" s="18"/>
+      <c r="AA4" s="18"/>
+      <c r="AB4" s="18"/>
+      <c r="AC4" s="18"/>
+      <c r="AD4" s="18"/>
+      <c r="AE4" s="18"/>
+      <c r="AF4" s="18"/>
+      <c r="AG4" s="18"/>
+      <c r="AH4" s="18"/>
+      <c r="AI4" s="18"/>
+      <c r="AJ4" s="18"/>
+      <c r="AK4" s="18"/>
+      <c r="AL4" s="18"/>
+      <c r="AM4" s="18"/>
+      <c r="AN4" s="18"/>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>1097</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="B5" s="13" t="s">
         <v>1110</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="C5" s="14" t="s">
         <v>1111</v>
       </c>
-      <c r="E4" s="15">
+      <c r="D5" s="15">
         <v>2</v>
       </c>
-      <c r="F4" s="15">
+      <c r="E5" s="15">
         <v>9.8000000000000007</v>
       </c>
-      <c r="G4" s="15">
+      <c r="F5" s="15">
         <v>8.5399999999999991</v>
       </c>
-      <c r="H4" s="15">
+      <c r="G5" s="15">
         <v>3.45</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15">
+      <c r="H5" s="15"/>
+      <c r="I5" s="15">
         <v>3.5</v>
       </c>
-      <c r="K4" s="15">
+      <c r="J5" s="15">
         <v>1.55</v>
       </c>
-      <c r="L4" s="15">
-        <f t="shared" ref="L4:L15" si="0">(J4*0.984) / (G4*3.28*0.01)^3</f>
+      <c r="K5" s="15">
+        <f t="shared" ref="K5:K17" si="0">(I5*0.984) / (F5*3.28*0.01)^3</f>
         <v>156.69964030781534</v>
       </c>
-      <c r="M4" s="15">
+      <c r="L5" s="15">
         <v>31</v>
       </c>
-      <c r="N4" s="15">
+      <c r="M5" s="15">
         <v>27</v>
       </c>
-      <c r="O4" s="15">
+      <c r="N5" s="15">
         <v>90</v>
       </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+      <c r="O5" s="19">
+        <f>MIN(S5:AN5)</f>
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="P5" s="19">
+        <f>MEDIAN(S5,AN5)</f>
+        <v>1.008</v>
+      </c>
+      <c r="Q5" s="19">
+        <f>MAX(S5:AN5)</f>
+        <v>1.008</v>
+      </c>
+      <c r="S5" s="18">
+        <v>1.008</v>
+      </c>
+      <c r="T5" s="18">
+        <v>1.008</v>
+      </c>
+      <c r="U5" s="18">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="V5" s="18"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="18"/>
+      <c r="AB5" s="18"/>
+      <c r="AC5" s="18"/>
+      <c r="AD5" s="18"/>
+      <c r="AE5" s="18"/>
+      <c r="AF5" s="18"/>
+      <c r="AG5" s="18"/>
+      <c r="AH5" s="18"/>
+      <c r="AI5" s="18"/>
+      <c r="AJ5" s="18"/>
+      <c r="AK5" s="18"/>
+      <c r="AL5" s="18"/>
+      <c r="AM5" s="18"/>
+      <c r="AN5" s="18"/>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D6" s="15">
+        <v>1.95</v>
+      </c>
+      <c r="E6" s="15">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="F6" s="15">
+        <v>8.4</v>
+      </c>
+      <c r="G6" s="15">
+        <v>3</v>
+      </c>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="J6" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="K6" s="15">
+        <f t="shared" si="0"/>
+        <v>89.390076729822283</v>
+      </c>
+      <c r="L6" s="15">
+        <v>25</v>
+      </c>
+      <c r="M6" s="15">
+        <v>19</v>
+      </c>
+      <c r="N6" s="15">
+        <v>60</v>
+      </c>
+      <c r="O6" s="19">
+        <f t="shared" ref="O6:O17" si="1">MIN(S6:AK6)</f>
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="P6" s="19">
+        <f t="shared" ref="P6:P17" si="2">MEDIAN(S6,AK6)</f>
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="Q6" s="19">
+        <f t="shared" ref="Q6:Q17" si="3">MAX(S6:AK6)</f>
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="S6" s="18">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="T6" s="18"/>
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="18"/>
+      <c r="AA6" s="18"/>
+      <c r="AB6" s="18"/>
+      <c r="AC6" s="18"/>
+      <c r="AD6" s="18"/>
+      <c r="AE6" s="18"/>
+      <c r="AF6" s="18"/>
+      <c r="AG6" s="18"/>
+      <c r="AH6" s="18"/>
+      <c r="AI6" s="18"/>
+      <c r="AJ6" s="18"/>
+      <c r="AK6" s="18"/>
+      <c r="AL6" s="18"/>
+      <c r="AM6" s="18"/>
+      <c r="AN6" s="18"/>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
         <v>1101</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="B7" s="13" t="s">
         <v>1114</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="C7" s="14" t="s">
         <v>1115</v>
       </c>
-      <c r="E5" s="15">
+      <c r="D7" s="15">
         <v>1.9</v>
       </c>
-      <c r="F5" s="15">
+      <c r="E7" s="15">
         <v>9.77</v>
       </c>
-      <c r="G5" s="15">
+      <c r="F7" s="15">
         <v>8.5500000000000007</v>
       </c>
-      <c r="H5" s="15">
+      <c r="G7" s="15">
         <v>3.48</v>
       </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15">
+      <c r="H7" s="15"/>
+      <c r="I7" s="15">
         <v>3.4</v>
       </c>
-      <c r="K5" s="15">
+      <c r="J7" s="15">
         <v>1.3</v>
       </c>
-      <c r="L5" s="15">
+      <c r="K7" s="15">
         <f t="shared" si="0"/>
         <v>151.68901811665376</v>
       </c>
-      <c r="M5" s="15">
+      <c r="L7" s="15">
         <v>34</v>
       </c>
-      <c r="N5" s="15">
+      <c r="M7" s="15">
         <v>30</v>
       </c>
-      <c r="O5" s="15">
+      <c r="N7" s="15">
         <v>83</v>
       </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+      <c r="O7" s="19">
+        <f t="shared" ref="O7:O17" si="4">MIN(S7:AN7)</f>
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="P7" s="19">
+        <f t="shared" ref="P7:P17" si="5">MEDIAN(S7,AN7)</f>
+        <v>0.995</v>
+      </c>
+      <c r="Q7" s="19">
+        <f t="shared" ref="Q7:Q17" si="6">MAX(S7:AN7)</f>
+        <v>1.006</v>
+      </c>
+      <c r="S7" s="18">
+        <v>0.995</v>
+      </c>
+      <c r="T7" s="18">
+        <v>0.997</v>
+      </c>
+      <c r="U7" s="18">
+        <v>1</v>
+      </c>
+      <c r="V7" s="18">
+        <v>0.99</v>
+      </c>
+      <c r="W7" s="18">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="X7" s="18">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="Y7" s="18">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="Z7" s="18">
+        <v>1.0029999999999999</v>
+      </c>
+      <c r="AA7" s="18">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="AB7" s="18">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="AC7" s="18">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="AD7" s="18">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="AE7" s="18">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="AF7" s="18">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="AG7" s="18">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="AH7" s="18">
+        <v>1.004</v>
+      </c>
+      <c r="AI7" s="18">
+        <v>0.998</v>
+      </c>
+      <c r="AJ7" s="18">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="AK7" s="18">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="AL7" s="18">
+        <v>1.006</v>
+      </c>
+      <c r="AM7" s="18">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="AN7" s="18"/>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>1098</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="B8" s="13" t="s">
         <v>1109</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="C8" s="14" t="s">
         <v>1112</v>
       </c>
-      <c r="E6" s="15">
+      <c r="D8" s="15">
         <v>2</v>
       </c>
-      <c r="F6" s="15">
+      <c r="E8" s="15">
         <v>10</v>
       </c>
-      <c r="G6" s="15">
+      <c r="F8" s="15">
         <v>8.76</v>
       </c>
-      <c r="H6" s="15">
+      <c r="G8" s="15">
         <v>3.39</v>
       </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15">
+      <c r="H8" s="15"/>
+      <c r="I8" s="15">
         <v>3.85</v>
       </c>
-      <c r="K6" s="15">
+      <c r="J8" s="15">
         <v>1.65</v>
       </c>
-      <c r="L6" s="15">
+      <c r="K8" s="15">
         <f t="shared" si="0"/>
         <v>159.7062742699336</v>
       </c>
-      <c r="M6" s="15">
+      <c r="L8" s="15">
         <v>33</v>
       </c>
-      <c r="N6" s="15">
+      <c r="M8" s="15">
         <v>25</v>
       </c>
-      <c r="O6" s="16" t="s">
+      <c r="N8" s="16" t="s">
         <v>1130</v>
       </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
+      <c r="O8" s="19">
+        <f t="shared" ref="O8:O17" si="7">MIN(S8:AK8)</f>
+        <v>0.995</v>
+      </c>
+      <c r="P8" s="19">
+        <f t="shared" ref="P8:P17" si="8">MEDIAN(S8,AK8)</f>
+        <v>1</v>
+      </c>
+      <c r="Q8" s="19">
+        <f t="shared" ref="Q8:Q17" si="9">MAX(S8:AK8)</f>
+        <v>1.008</v>
+      </c>
+      <c r="S8" s="18">
+        <v>1</v>
+      </c>
+      <c r="T8" s="18">
+        <v>1.002</v>
+      </c>
+      <c r="U8" s="18">
+        <v>1</v>
+      </c>
+      <c r="V8" s="18">
+        <v>1.002</v>
+      </c>
+      <c r="W8" s="18">
+        <v>0.995</v>
+      </c>
+      <c r="X8" s="18">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="Y8" s="18">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="Z8" s="18">
+        <v>1.008</v>
+      </c>
+      <c r="AA8" s="18">
+        <v>0.998</v>
+      </c>
+      <c r="AB8" s="18">
+        <v>1.006</v>
+      </c>
+      <c r="AC8" s="18"/>
+      <c r="AD8" s="18"/>
+      <c r="AE8" s="18"/>
+      <c r="AF8" s="18"/>
+      <c r="AG8" s="18"/>
+      <c r="AH8" s="18"/>
+      <c r="AI8" s="18"/>
+      <c r="AJ8" s="18"/>
+      <c r="AK8" s="18"/>
+      <c r="AL8" s="18"/>
+      <c r="AM8" s="18"/>
+      <c r="AN8" s="18"/>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
         <v>1102</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="B9" s="13" t="s">
         <v>1114</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="C9" s="14" t="s">
         <v>1116</v>
       </c>
-      <c r="E7" s="15">
+      <c r="D9" s="15">
         <v>2.13</v>
       </c>
-      <c r="F7" s="15">
+      <c r="E9" s="15">
         <v>10.8</v>
       </c>
-      <c r="G7" s="15">
+      <c r="F9" s="15">
         <v>9.5</v>
       </c>
-      <c r="H7" s="15">
+      <c r="G9" s="15">
         <v>3.55</v>
       </c>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15">
+      <c r="H9" s="15"/>
+      <c r="I9" s="15">
         <v>4.9000000000000004</v>
       </c>
-      <c r="K7" s="15">
+      <c r="J9" s="15">
         <v>2</v>
       </c>
-      <c r="L7" s="15">
+      <c r="K9" s="15">
         <f t="shared" si="0"/>
         <v>159.36715929838209</v>
       </c>
-      <c r="M7" s="15">
+      <c r="L9" s="15">
         <v>37</v>
       </c>
-      <c r="N7" s="15">
+      <c r="M9" s="15">
         <v>33</v>
       </c>
-      <c r="O7" s="15">
+      <c r="N9" s="15">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
+      <c r="O9" s="19">
+        <f t="shared" ref="O9:O17" si="10">MIN(S9:AN9)</f>
+        <v>1.022</v>
+      </c>
+      <c r="P9" s="19">
+        <f t="shared" ref="P9:P17" si="11">MEDIAN(S9,AN9)</f>
+        <v>1.0389999999999999</v>
+      </c>
+      <c r="Q9" s="19">
+        <f t="shared" ref="Q9:Q17" si="12">MAX(S9:AN9)</f>
+        <v>1.042</v>
+      </c>
+      <c r="S9" s="18">
+        <v>1.0389999999999999</v>
+      </c>
+      <c r="T9" s="18">
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="U9" s="18">
+        <v>1.022</v>
+      </c>
+      <c r="V9" s="18">
+        <v>1.038</v>
+      </c>
+      <c r="W9" s="18">
+        <v>1.04</v>
+      </c>
+      <c r="X9" s="18">
+        <v>1.042</v>
+      </c>
+      <c r="Y9" s="18">
+        <v>1.0369999999999999</v>
+      </c>
+      <c r="Z9" s="18">
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="AA9" s="18"/>
+      <c r="AB9" s="18"/>
+      <c r="AC9" s="18"/>
+      <c r="AD9" s="18"/>
+      <c r="AE9" s="18"/>
+      <c r="AF9" s="18"/>
+      <c r="AG9" s="18"/>
+      <c r="AH9" s="18"/>
+      <c r="AI9" s="18"/>
+      <c r="AJ9" s="18"/>
+      <c r="AK9" s="18"/>
+      <c r="AL9" s="18"/>
+      <c r="AM9" s="18"/>
+      <c r="AN9" s="18"/>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>1099</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="B10" s="13" t="s">
         <v>1109</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="C10" s="14" t="s">
         <v>1113</v>
       </c>
-      <c r="E8" s="15">
+      <c r="D10" s="15">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F8" s="15">
+      <c r="E10" s="15">
         <v>10.8</v>
       </c>
-      <c r="G8" s="15">
+      <c r="F10" s="15">
         <v>9.4</v>
       </c>
-      <c r="H8" s="15">
+      <c r="G10" s="15">
         <v>3.65</v>
       </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15">
+      <c r="H10" s="15"/>
+      <c r="I10" s="15">
         <v>4.75</v>
       </c>
-      <c r="K8" s="15">
+      <c r="J10" s="15">
         <v>2.15</v>
       </c>
-      <c r="L8" s="15">
+      <c r="K10" s="15">
         <f t="shared" si="0"/>
         <v>159.4716971374134</v>
       </c>
-      <c r="M8" s="15">
+      <c r="L10" s="15">
         <v>40</v>
       </c>
-      <c r="N8" s="15">
+      <c r="M10" s="15">
         <v>33</v>
       </c>
-      <c r="O8" s="16" t="s">
+      <c r="N10" s="16" t="s">
         <v>1131</v>
       </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
+      <c r="O10" s="19">
+        <f t="shared" ref="O10:O17" si="13">MIN(S10:AK10)</f>
+        <v>1.034</v>
+      </c>
+      <c r="P10" s="19">
+        <f t="shared" ref="P10:P17" si="14">MEDIAN(S10,AK10)</f>
+        <v>1.0389999999999999</v>
+      </c>
+      <c r="Q10" s="19">
+        <f t="shared" ref="Q10:Q17" si="15">MAX(S10:AK10)</f>
+        <v>1.046</v>
+      </c>
+      <c r="S10" s="18">
+        <v>1.0389999999999999</v>
+      </c>
+      <c r="T10" s="18">
+        <v>1.0369999999999999</v>
+      </c>
+      <c r="U10" s="18">
+        <v>1.034</v>
+      </c>
+      <c r="V10" s="18">
+        <v>1.0369999999999999</v>
+      </c>
+      <c r="W10" s="18">
+        <v>1.038</v>
+      </c>
+      <c r="X10" s="18">
+        <v>1.046</v>
+      </c>
+      <c r="Y10" s="18"/>
+      <c r="Z10" s="18"/>
+      <c r="AA10" s="18"/>
+      <c r="AB10" s="18"/>
+      <c r="AC10" s="18"/>
+      <c r="AD10" s="18"/>
+      <c r="AE10" s="18"/>
+      <c r="AF10" s="18"/>
+      <c r="AG10" s="18"/>
+      <c r="AH10" s="18"/>
+      <c r="AI10" s="18"/>
+      <c r="AJ10" s="18"/>
+      <c r="AK10" s="18"/>
+      <c r="AL10" s="18"/>
+      <c r="AM10" s="18"/>
+      <c r="AN10" s="18"/>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>1119</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="B11" s="13" t="s">
         <v>1120</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15" t="s">
+      <c r="C11" s="14"/>
+      <c r="D11" s="15" t="s">
         <v>1125</v>
       </c>
-      <c r="F9" s="15">
+      <c r="E11" s="15">
         <v>10.5</v>
       </c>
-      <c r="G9" s="15">
+      <c r="F11" s="15">
         <v>10.5</v>
       </c>
-      <c r="H9" s="15">
+      <c r="G11" s="15">
         <v>3.9</v>
       </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15">
+      <c r="H11" s="15"/>
+      <c r="I11" s="15">
         <v>3.6</v>
       </c>
-      <c r="K9" s="15">
+      <c r="J11" s="15">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L9" s="15">
+      <c r="K11" s="15">
         <f t="shared" si="0"/>
         <v>86.717783909688649</v>
       </c>
-      <c r="M9" s="15">
+      <c r="L11" s="15">
         <v>37</v>
       </c>
-      <c r="N9" s="15">
+      <c r="M11" s="15">
         <v>34</v>
       </c>
-      <c r="O9" s="15">
+      <c r="N11" s="15">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
+      <c r="O11" s="19">
+        <f t="shared" ref="O11:O17" si="16">MIN(S11:AN11)</f>
+        <v>1.0820000000000001</v>
+      </c>
+      <c r="P11" s="19">
+        <f t="shared" ref="P11:P17" si="17">MEDIAN(S11,AN11)</f>
+        <v>1.0820000000000001</v>
+      </c>
+      <c r="Q11" s="19">
+        <f t="shared" ref="Q11:Q17" si="18">MAX(S11:AN11)</f>
+        <v>1.0820000000000001</v>
+      </c>
+      <c r="S11" s="20">
+        <v>1.0820000000000001</v>
+      </c>
+      <c r="T11" s="18"/>
+      <c r="U11" s="18"/>
+      <c r="V11" s="18"/>
+      <c r="W11" s="18"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="18"/>
+      <c r="Z11" s="18"/>
+      <c r="AA11" s="18"/>
+      <c r="AB11" s="18"/>
+      <c r="AC11" s="18"/>
+      <c r="AD11" s="18"/>
+      <c r="AE11" s="18"/>
+      <c r="AF11" s="18"/>
+      <c r="AG11" s="18"/>
+      <c r="AH11" s="18"/>
+      <c r="AI11" s="18"/>
+      <c r="AJ11" s="18"/>
+      <c r="AK11" s="18"/>
+      <c r="AL11" s="18"/>
+      <c r="AM11" s="18"/>
+      <c r="AN11" s="18"/>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>1117</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="B12" s="13" t="s">
         <v>1120</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="C12" s="14" t="s">
         <v>1121</v>
       </c>
-      <c r="E10" s="15">
+      <c r="D12" s="15">
         <v>1.6</v>
       </c>
-      <c r="F10" s="15">
+      <c r="E12" s="15">
         <v>9.14</v>
       </c>
-      <c r="G10" s="15">
+      <c r="F12" s="15">
         <v>9.1</v>
       </c>
-      <c r="H10" s="15">
+      <c r="G12" s="15">
         <v>3.7</v>
       </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15">
+      <c r="H12" s="15"/>
+      <c r="I12" s="15">
         <v>2.8</v>
       </c>
-      <c r="K10" s="15">
+      <c r="J12" s="15">
         <v>0.95</v>
       </c>
-      <c r="L10" s="15">
+      <c r="K12" s="15">
         <f t="shared" si="0"/>
         <v>103.61137130766168</v>
       </c>
-      <c r="M10" s="15">
+      <c r="L12" s="15">
         <v>34</v>
       </c>
-      <c r="N10" s="15">
+      <c r="M12" s="15">
         <v>26</v>
       </c>
-      <c r="O10" s="15">
+      <c r="N12" s="15">
         <v>92</v>
       </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="13" t="s">
+      <c r="O12" s="19">
+        <f t="shared" ref="O12:O17" si="19">MIN(S12:AK12)</f>
+        <v>1.002</v>
+      </c>
+      <c r="P12" s="19">
+        <f t="shared" ref="P12:P17" si="20">MEDIAN(S12,AK12)</f>
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="Q12" s="19">
+        <f t="shared" ref="Q12:Q17" si="21">MAX(S12:AK12)</f>
+        <v>1.038</v>
+      </c>
+      <c r="S12" s="18">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="T12" s="18">
+        <v>1.038</v>
+      </c>
+      <c r="U12" s="18">
+        <v>1.002</v>
+      </c>
+      <c r="V12" s="18">
+        <v>1.0129999999999999</v>
+      </c>
+      <c r="W12" s="18">
+        <v>1.0109999999999999</v>
+      </c>
+      <c r="X12" s="18">
+        <v>1.018</v>
+      </c>
+      <c r="Y12" s="18">
+        <v>1.0209999999999999</v>
+      </c>
+      <c r="Z12" s="18">
+        <v>1.0189999999999999</v>
+      </c>
+      <c r="AA12" s="18"/>
+      <c r="AB12" s="18"/>
+      <c r="AC12" s="18"/>
+      <c r="AD12" s="18"/>
+      <c r="AE12" s="18"/>
+      <c r="AF12" s="18"/>
+      <c r="AG12" s="18"/>
+      <c r="AH12" s="18"/>
+      <c r="AI12" s="18"/>
+      <c r="AJ12" s="18"/>
+      <c r="AK12" s="18"/>
+      <c r="AL12" s="18"/>
+      <c r="AM12" s="18"/>
+      <c r="AN12" s="18"/>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
         <v>1118</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="B13" s="21" t="s">
         <v>1120</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="C13" s="22" t="s">
         <v>1122</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="D13" s="23" t="s">
         <v>1123</v>
       </c>
-      <c r="F11" s="15">
+      <c r="E13" s="23">
         <v>10.8</v>
       </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15">
+      <c r="F13" s="23">
+        <v>10</v>
+      </c>
+      <c r="G13" s="23">
         <v>4</v>
       </c>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15">
+      <c r="H13" s="23"/>
+      <c r="I13" s="23">
         <v>4</v>
       </c>
-      <c r="K11" s="15">
+      <c r="J13" s="23">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L11" s="15" t="e">
+      <c r="K13" s="23">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M11" s="15">
+        <v>111.54074955383705</v>
+      </c>
+      <c r="L13" s="23">
         <v>45</v>
       </c>
-      <c r="N11" s="15">
-        <v>29</v>
-      </c>
-      <c r="O11" s="16" t="s">
+      <c r="M13" s="23">
+        <v>39</v>
+      </c>
+      <c r="N13" s="25" t="s">
         <v>1134</v>
       </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
+      <c r="O13" s="24">
+        <f t="shared" ref="O13:O17" si="22">MIN(S13:AN13)</f>
+        <v>1.117</v>
+      </c>
+      <c r="P13" s="24">
+        <f t="shared" ref="P13:P17" si="23">MEDIAN(S13,AN13)</f>
+        <v>1.117</v>
+      </c>
+      <c r="Q13" s="24">
+        <f t="shared" ref="Q13:Q17" si="24">MAX(S13:AN13)</f>
+        <v>1.117</v>
+      </c>
+      <c r="S13" s="20">
+        <v>1.117</v>
+      </c>
+      <c r="T13" s="18"/>
+      <c r="U13" s="18"/>
+      <c r="V13" s="18"/>
+      <c r="W13" s="18"/>
+      <c r="X13" s="18"/>
+      <c r="Y13" s="18"/>
+      <c r="Z13" s="18"/>
+      <c r="AA13" s="18"/>
+      <c r="AB13" s="18"/>
+      <c r="AC13" s="18"/>
+      <c r="AD13" s="18"/>
+      <c r="AE13" s="18"/>
+      <c r="AF13" s="18"/>
+      <c r="AG13" s="18"/>
+      <c r="AH13" s="18"/>
+      <c r="AI13" s="18"/>
+      <c r="AJ13" s="18"/>
+      <c r="AK13" s="18"/>
+      <c r="AL13" s="18"/>
+      <c r="AM13" s="18"/>
+      <c r="AN13" s="18"/>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>1138</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15">
+      <c r="B14" s="13"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="15">
         <v>2.4</v>
       </c>
-      <c r="F12" s="15">
+      <c r="E14" s="15">
         <v>9.9</v>
       </c>
-      <c r="G12" s="15">
+      <c r="F14" s="15">
         <v>9.9</v>
       </c>
-      <c r="H12" s="15">
+      <c r="G14" s="15">
         <v>3</v>
       </c>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15">
+      <c r="H14" s="15"/>
+      <c r="I14" s="15">
         <v>2.7</v>
       </c>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15">
+      <c r="J14" s="15"/>
+      <c r="K14" s="15">
         <f t="shared" si="0"/>
         <v>77.594644484679435</v>
       </c>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="16"/>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="s">
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="19">
+        <f t="shared" ref="O14:O17" si="25">MIN(S14:AK14)</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="P14" s="19">
+        <f t="shared" ref="P14:P17" si="26">MEDIAN(S14,AK14)</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="Q14" s="19">
+        <f t="shared" ref="Q14:Q17" si="27">MAX(S14:AK14)</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="S14" s="18">
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="T14" s="18"/>
+      <c r="U14" s="18"/>
+      <c r="V14" s="18"/>
+      <c r="W14" s="18"/>
+      <c r="X14" s="18"/>
+      <c r="Y14" s="18"/>
+      <c r="Z14" s="18"/>
+      <c r="AA14" s="18"/>
+      <c r="AB14" s="18"/>
+      <c r="AC14" s="18"/>
+      <c r="AD14" s="18"/>
+      <c r="AE14" s="18"/>
+      <c r="AF14" s="18"/>
+      <c r="AG14" s="18"/>
+      <c r="AH14" s="18"/>
+      <c r="AI14" s="18"/>
+      <c r="AJ14" s="18"/>
+      <c r="AK14" s="18"/>
+      <c r="AL14" s="18"/>
+      <c r="AM14" s="18"/>
+      <c r="AN14" s="18"/>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
         <v>1139</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="B15" s="13" t="s">
         <v>1140</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="15">
+      <c r="C15" s="14"/>
+      <c r="D15" s="15">
         <v>2.1</v>
       </c>
-      <c r="F13" s="15">
+      <c r="E15" s="15">
         <v>12</v>
       </c>
-      <c r="G13" s="15">
+      <c r="F15" s="15">
         <v>10.3</v>
       </c>
-      <c r="H13" s="15">
+      <c r="G15" s="15">
         <v>3.8</v>
       </c>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15">
+      <c r="H15" s="15"/>
+      <c r="I15" s="15">
         <v>4.3</v>
       </c>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15">
+      <c r="J15" s="15"/>
+      <c r="K15" s="15">
         <f t="shared" si="0"/>
         <v>109.73125562960811</v>
       </c>
-      <c r="M13" s="15">
+      <c r="L15" s="15">
         <v>41</v>
       </c>
-      <c r="N13" s="15">
+      <c r="M15" s="15">
         <v>28</v>
       </c>
-      <c r="O13" s="16"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="13" t="s">
+      <c r="N15" s="16"/>
+      <c r="O15" s="19">
+        <f t="shared" ref="O15:O17" si="28">MIN(S15:AN15)</f>
+        <v>1.0309999999999999</v>
+      </c>
+      <c r="P15" s="19">
+        <f t="shared" ref="P15:P17" si="29">MEDIAN(S15,AN15)</f>
+        <v>1.0309999999999999</v>
+      </c>
+      <c r="Q15" s="19">
+        <f t="shared" ref="Q15:Q17" si="30">MAX(S15:AN15)</f>
+        <v>1.0309999999999999</v>
+      </c>
+      <c r="S15" s="18">
+        <v>1.0309999999999999</v>
+      </c>
+      <c r="T15" s="18"/>
+      <c r="U15" s="18"/>
+      <c r="V15" s="18"/>
+      <c r="W15" s="18"/>
+      <c r="X15" s="18"/>
+      <c r="Y15" s="18"/>
+      <c r="Z15" s="18"/>
+      <c r="AA15" s="18"/>
+      <c r="AB15" s="18"/>
+      <c r="AC15" s="18"/>
+      <c r="AD15" s="18"/>
+      <c r="AE15" s="18"/>
+      <c r="AF15" s="18"/>
+      <c r="AG15" s="18"/>
+      <c r="AH15" s="18"/>
+      <c r="AI15" s="18"/>
+      <c r="AJ15" s="18"/>
+      <c r="AK15" s="18"/>
+      <c r="AL15" s="18"/>
+      <c r="AM15" s="18"/>
+      <c r="AN15" s="18"/>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
         <v>1132</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="B16" s="13" t="s">
         <v>1110</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="15">
+      <c r="C16" s="14"/>
+      <c r="D16" s="15">
         <v>2.15</v>
       </c>
-      <c r="F14" s="15">
+      <c r="E16" s="15">
         <v>10.11</v>
       </c>
-      <c r="G14" s="15">
+      <c r="F16" s="15">
         <v>9.82</v>
       </c>
-      <c r="H14" s="15">
+      <c r="G16" s="15">
         <v>3.43</v>
       </c>
-      <c r="I14" s="15">
+      <c r="H16" s="15">
         <v>2.5</v>
       </c>
-      <c r="J14" s="15">
+      <c r="I16" s="15">
         <v>3</v>
       </c>
-      <c r="K14" s="15">
+      <c r="J16" s="15">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L14" s="15">
+      <c r="K16" s="15">
         <f t="shared" si="0"/>
         <v>88.340602856022727</v>
       </c>
-      <c r="M14" s="15">
+      <c r="L16" s="15">
         <v>38</v>
       </c>
-      <c r="N14" s="15">
+      <c r="M16" s="15">
         <v>30</v>
       </c>
-      <c r="O14" s="15">
+      <c r="N16" s="15">
         <v>85</v>
       </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
+      <c r="O16" s="19">
+        <f t="shared" ref="O16:O17" si="31">MIN(S16:AK16)</f>
+        <v>1.046</v>
+      </c>
+      <c r="P16" s="19">
+        <f t="shared" ref="P16:P17" si="32">MEDIAN(S16,AK16)</f>
+        <v>1.046</v>
+      </c>
+      <c r="Q16" s="19">
+        <f t="shared" ref="Q16:Q17" si="33">MAX(S16:AK16)</f>
+        <v>1.105</v>
+      </c>
+      <c r="S16" s="18">
+        <v>1.046</v>
+      </c>
+      <c r="T16" s="20">
+        <v>1.097</v>
+      </c>
+      <c r="U16" s="20">
+        <v>1.0609999999999999</v>
+      </c>
+      <c r="V16" s="20">
+        <v>1.085</v>
+      </c>
+      <c r="W16" s="20">
+        <v>1.0920000000000001</v>
+      </c>
+      <c r="X16" s="20">
+        <v>1.105</v>
+      </c>
+      <c r="Y16" s="20">
+        <v>1.091</v>
+      </c>
+      <c r="Z16" s="20">
+        <v>1.0609999999999999</v>
+      </c>
+      <c r="AA16" s="20">
+        <v>1.0609999999999999</v>
+      </c>
+      <c r="AB16" s="20">
+        <v>1.0660000000000001</v>
+      </c>
+      <c r="AC16" s="18"/>
+      <c r="AD16" s="18"/>
+      <c r="AE16" s="18"/>
+      <c r="AF16" s="18"/>
+      <c r="AG16" s="18"/>
+      <c r="AH16" s="18"/>
+      <c r="AI16" s="18"/>
+      <c r="AJ16" s="18"/>
+      <c r="AK16" s="18"/>
+      <c r="AL16" s="18"/>
+      <c r="AM16" s="18"/>
+      <c r="AN16" s="18"/>
+    </row>
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
         <v>1135</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="B17" s="21" t="s">
         <v>1136</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15">
+      <c r="C17" s="22"/>
+      <c r="D17" s="23">
         <v>1.8</v>
       </c>
-      <c r="F15" s="15">
+      <c r="E17" s="23">
         <v>9.1999999999999993</v>
       </c>
-      <c r="G15" s="15">
+      <c r="F17" s="23">
         <v>8.4</v>
       </c>
-      <c r="H15" s="15">
+      <c r="G17" s="23">
         <v>3.25</v>
       </c>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15">
+      <c r="H17" s="23"/>
+      <c r="I17" s="23">
         <v>2.5</v>
       </c>
-      <c r="K15" s="15">
+      <c r="J17" s="23">
         <v>0.9</v>
       </c>
-      <c r="L15" s="15">
+      <c r="K17" s="23">
         <f t="shared" si="0"/>
         <v>117.61852201292405</v>
       </c>
-      <c r="M15" s="15">
+      <c r="L17" s="23">
         <v>26</v>
       </c>
-      <c r="N15" s="15">
+      <c r="M17" s="23">
         <v>30</v>
       </c>
-      <c r="O15" s="15">
+      <c r="N17" s="23">
         <v>73</v>
       </c>
+      <c r="O17" s="24">
+        <f t="shared" ref="O17" si="34">MIN(S17:AN17)</f>
+        <v>9.6299999999999997E-2</v>
+      </c>
+      <c r="P17" s="24">
+        <f t="shared" ref="P17" si="35">MEDIAN(S17,AN17)</f>
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="Q17" s="24">
+        <f t="shared" ref="Q17" si="36">MAX(S17:AN17)</f>
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="S17" s="20">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="T17" s="20">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="U17" s="20">
+        <v>9.6299999999999997E-2</v>
+      </c>
+      <c r="V17" s="20">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="W17" s="18"/>
+      <c r="X17" s="18"/>
+      <c r="Y17" s="18"/>
+      <c r="Z17" s="18"/>
+      <c r="AA17" s="18"/>
+      <c r="AB17" s="18"/>
+      <c r="AC17" s="18"/>
+      <c r="AD17" s="18"/>
+      <c r="AE17" s="18"/>
+      <c r="AF17" s="18"/>
+      <c r="AG17" s="18"/>
+      <c r="AH17" s="18"/>
+      <c r="AI17" s="18"/>
+      <c r="AJ17" s="18"/>
+      <c r="AK17" s="18"/>
+      <c r="AL17" s="18"/>
+      <c r="AM17" s="18"/>
+      <c r="AN17" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>